<commit_message>
ok add zek items
</commit_message>
<xml_diff>
--- a/Elin_SukutsuArena/LangMod/EN/SourceChara.xlsx
+++ b/Elin_SukutsuArena/LangMod/EN/SourceChara.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="350" uniqueCount="211">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="353" uniqueCount="212">
   <si>
     <t xml:space="preserve">id</t>
   </si>
@@ -223,7 +223,7 @@
     <t xml:space="preserve">neutral,addZone_sukutsu_arena,addFlag_StayHomeZone,addStock_sukutsu_receptionist,addDrama_drama_sukutsu_receptionist,humanSpeak</t>
   </si>
   <si>
-    <t xml:space="preserve">Merchant</t>
+    <t xml:space="preserve">SukutsuMerchant</t>
   </si>
   <si>
     <t xml:space="preserve">succubus</t>
@@ -256,7 +256,10 @@
     <t xml:space="preserve">neutral,addZone_sukutsu_arena,addFlag_StayHomeZone,addDrama_drama_sukutsu_arena_master,humanSpeak</t>
   </si>
   <si>
-    <t xml:space="preserve">human</t>
+    <t xml:space="preserve">SukutsuNPC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">juere</t>
   </si>
   <si>
     <t xml:space="preserve">warrior</t>
@@ -286,13 +289,13 @@
     <t xml:space="preserve">dragon</t>
   </si>
   <si>
-    <t xml:space="preserve">breathe_Void/40,breathe_Chaos/30,breathe_Nether/25,hand_Magic/35,SpGravity/15,SpBane/10</t>
+    <t xml:space="preserve">breathe_Void/35,breathe_Chaos/25,breathe_Nether/20,hand_Magic/30,SpGravity/10,SpBane/5,ActGazeInsane/15,ActGazeMutation/10,ActCurse/10,ActBurnMana/15,SpHeal/5,SpSummonDragon/5,SpEarthquake/5,SpShutterHex/5,SpSpeedDown/5,SpSilence/5,SpWeakness/5,SpNightmare/5,SpSummonTentacle/5,SpGate/5,ActTouchDrown/5,ActNeckHunt/5</t>
   </si>
   <si>
     <t xml:space="preserve">Void</t>
   </si>
   <si>
-    <t xml:space="preserve">featElder/1,featBodyParts/12,resVoid/100,resChaos/80,resNether/80,resMagic/80,resDarkness/80,resFire/60,resCold/60,resLightning/60,resPoison/60,resAcid/60,resSound/60,resNerve/80,resMind/80,resHoly/40,resCut/50,resImpact/50</t>
+    <t xml:space="preserve">featElder/1,featBodyParts/12,resVoid/20,resChaos/20,resNether/20,resMagic/20,resDarkness/20,resFire/20,resNerve/20,resMind/20,resHoly/20,resCut/20,resImpact/20,featBoost/1,featBloodBond/1</t>
   </si>
   <si>
     <t xml:space="preserve">m/1003/350/500/proud</t>
@@ -304,7 +307,7 @@
     <t xml:space="preserve">sukutsu_shady_merchant</t>
   </si>
   <si>
-    <t xml:space="preserve">エゼキエル</t>
+    <t xml:space="preserve">ゼク</t>
   </si>
   <si>
     <t xml:space="preserve">Ezekiel</t>
@@ -379,13 +382,13 @@
     <t xml:space="preserve">slime</t>
   </si>
   <si>
-    <t xml:space="preserve">breathe_Chaos/30</t>
+    <t xml:space="preserve">breathe_Chaos/30,ActStealFood/15,ActStealMoney/15,ActDraw/10,ActTouchDrown/10</t>
   </si>
   <si>
     <t xml:space="preserve">Chaos</t>
   </si>
   <si>
-    <t xml:space="preserve">resChaos/100</t>
+    <t xml:space="preserve">resChaos/100,featMeatCushion/4</t>
   </si>
   <si>
     <t xml:space="preserve">n/2001/50/30/mindless</t>
@@ -430,9 +433,6 @@
     <t xml:space="preserve">百戦の覇者</t>
   </si>
   <si>
-    <t xml:space="preserve">breathe_Cut/30,breathe_Impact/20</t>
-  </si>
-  <si>
     <t xml:space="preserve">Cut</t>
   </si>
   <si>
@@ -454,10 +454,10 @@
     <t xml:space="preserve">Iron-Blooded Champion</t>
   </si>
   <si>
-    <t xml:space="preserve">breathe_Cut/45,breathe_Impact/35,SpHero/10</t>
-  </si>
-  <si>
-    <t xml:space="preserve">featElder/1,featBodyParts/8,resCut/80,resImpact/80,resFire/40,resCold/40,resLightning/40,resMind/60,resNerve/60</t>
+    <t xml:space="preserve">breathe_Cut/40,breathe_Impact/30,SpHero/10,ActRush/25,ActBash/20</t>
+  </si>
+  <si>
+    <t xml:space="preserve">featElder/1,featBodyParts/8,resCut/80,resImpact/80,resFire/40,resCold/40,resLightning/40,resMind/60,resNerve/60,antiMagic/60,vopal/60,mod_flurry/65,mod_chaser/30,mod_cleave/10,redirect_blaser/23,counter/20</t>
   </si>
   <si>
     <t xml:space="preserve">m/1002/188/95/stern</t>
@@ -481,13 +481,13 @@
     <t xml:space="preserve">boss,undead</t>
   </si>
   <si>
-    <t xml:space="preserve">chaos</t>
-  </si>
-  <si>
-    <t xml:space="preserve">breathe_Acid/25,breathe_Cut/25,hand_Nether/30</t>
-  </si>
-  <si>
-    <t xml:space="preserve">featBodyParts/5</t>
+    <t xml:space="preserve">wraith</t>
+  </si>
+  <si>
+    <t xml:space="preserve">breathe_Acid/25,breathe_Cut/25,hand_Nether/30,SpSummonShadow/15</t>
+  </si>
+  <si>
+    <t xml:space="preserve">featBodyParts/5,featUndead/1</t>
   </si>
   <si>
     <t xml:space="preserve">m/1006/180/0/melancholic</t>
@@ -499,9 +499,6 @@
     <t xml:space="preserve">Nul</t>
   </si>
   <si>
-    <t xml:space="preserve">Null</t>
-  </si>
-  <si>
     <t xml:space="preserve">虚無の処刑人</t>
   </si>
   <si>
@@ -517,13 +514,13 @@
     <t xml:space="preserve">thief</t>
   </si>
   <si>
-    <t xml:space="preserve">hand_Void/45,SpInvisibility/25,SpSilence/15</t>
-  </si>
-  <si>
-    <t xml:space="preserve">invisibility/1,featSplit/1,featElder/1,resVoid/80,resNether/60,resMagic/40,resNerve/100,resMind/100</t>
-  </si>
-  <si>
-    <t xml:space="preserve">f/1007/165/45/emotionless</t>
+    <t xml:space="preserve">hand_Void/40,SpInvisibility/30,SpSilence/15,ActGazeInsane/15,ActRush/10,ActInsult/10,SpEarthquake/10,SpSeeInvisible/10,arrow_Void/20</t>
+  </si>
+  <si>
+    <t xml:space="preserve">invisibility/1,featSplit/1,featElder/1,resVoid/80,resNether/60,resMagic/40,resNerve/100,resMind/100,featGolem/1,featReboot/1,featBoost/1,featEarthStrength/1,featRapidArrow/3,featGeneSlot/10,featMiscreation/1,featMetal/120,featManaMeat/1,featRoran/1,evasionPerfect/60</t>
+  </si>
+  <si>
+    <t xml:space="preserve">f/1007/165/45/princess</t>
   </si>
   <si>
     <t xml:space="preserve">UN_sukutsu_null</t>
@@ -544,7 +541,13 @@
     <t xml:space="preserve">Mirror Image</t>
   </si>
   <si>
-    <t xml:space="preserve">shade</t>
+    <t xml:space="preserve">phantom</t>
+  </si>
+  <si>
+    <t xml:space="preserve">arrow_Darkness/25,SpHeal/15,SpTeleport/15,ActSwarm/20,ActBladeStorm/20</t>
+  </si>
+  <si>
+    <t xml:space="preserve">featDemon/1</t>
   </si>
   <si>
     <t xml:space="preserve">n/1008/170/60/sinister</t>
@@ -565,13 +568,13 @@
     <t xml:space="preserve">Voice of the Audience</t>
   </si>
   <si>
-    <t xml:space="preserve">breathe_Sound/35,breathe_Chaos/25,SpWeakness/15</t>
+    <t xml:space="preserve">breathe_Sound/35,breathe_Chaos/25,SpWeakness/15,ActInsult/30,SpHeal/10</t>
   </si>
   <si>
     <t xml:space="preserve">Sound</t>
   </si>
   <si>
-    <t xml:space="preserve">resSound/50,resChaos/30,resMagic/60,featElder/1</t>
+    <t xml:space="preserve">resSound/50,resChaos/30,resMagic/60,featElder/1,featCosmicHorror/1</t>
   </si>
   <si>
     <t xml:space="preserve">m/2003/175/70/possessed</t>
@@ -896,15 +899,15 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="0" width="7.83"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="20" style="0" width="6.02"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="21" min="21" style="0" width="125.25"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="22" min="22" style="0" width="7.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="22" min="22" style="0" width="15.76"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="23" min="23" style="0" width="9.36"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="24" min="24" style="0" width="10.89"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="25" min="25" style="0" width="7"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="26" min="26" style="0" width="5.88"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="27" min="27" style="0" width="8.25"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="28" min="28" style="0" width="78.51"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="28" min="28" style="0" width="290.82"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="29" min="29" style="0" width="12.15"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="30" min="30" style="0" width="190.37"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="30" min="30" style="0" width="221.4"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="31" min="31" style="0" width="6.02"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="32" min="32" style="0" width="7.14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="33" min="33" style="0" width="8.52"/>
@@ -914,7 +917,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="37" min="37" style="0" width="7.14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="38" min="38" style="0" width="8.67"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="39" min="39" style="0" width="7.27"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="40" min="40" style="0" width="22.86"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="40" min="40" style="0" width="22.72"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="41" min="41" style="0" width="6.02"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="43" min="42" style="0" width="7.14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="44" min="44" style="0" width="21.04"/>
@@ -1360,14 +1363,17 @@
       <c r="U5" s="1" t="s">
         <v>77</v>
       </c>
+      <c r="V5" s="1" t="s">
+        <v>78</v>
+      </c>
       <c r="W5" s="1" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="X5" s="1" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="AN5" s="1" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="AR5" s="1" t="s">
         <v>72</v>
@@ -1378,19 +1384,19 @@
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="E6" s="0" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="J6" s="1" t="s">
         <v>64</v>
@@ -1411,51 +1417,51 @@
         <v>65</v>
       </c>
       <c r="U6" s="1" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="W6" s="1" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="X6" s="1" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="AB6" s="1" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="AC6" s="1" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="AD6" s="1" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="AN6" s="1" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="AR6" s="1" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="AML6" s="1" t="s">
         <v>71</v>
       </c>
       <c r="AMM6" s="1" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="E7" s="0" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="J7" s="1" t="s">
         <v>64</v>
@@ -1476,22 +1482,22 @@
         <v>65</v>
       </c>
       <c r="U7" s="1" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="V7" s="1" t="s">
         <v>67</v>
       </c>
       <c r="W7" s="1" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="X7" s="1" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="AN7" s="1" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="AR7" s="1" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="AML7" s="1" t="s">
         <v>71</v>
@@ -1499,19 +1505,19 @@
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="C8" s="0" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="E8" s="0" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="J8" s="1" t="s">
         <v>64</v>
@@ -1532,19 +1538,19 @@
         <v>65</v>
       </c>
       <c r="U8" s="1" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="W8" s="1" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="X8" s="1" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="AN8" s="1" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="AR8" s="1" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="AML8" s="1" t="s">
         <v>71</v>
@@ -1552,19 +1558,19 @@
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="C9" s="0" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="E9" s="0" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="J9" s="1" t="s">
         <v>64</v>
@@ -1582,31 +1588,31 @@
         <v>3</v>
       </c>
       <c r="S9" s="1" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="U9" s="1" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="W9" s="1" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="X9" s="1" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="AB9" s="1" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="AC9" s="1" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="AD9" s="1" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="AN9" s="1" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="AR9" s="1" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="AML9" s="1" t="s">
         <v>71</v>
@@ -1614,19 +1620,19 @@
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="C10" s="0" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="E10" s="0" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="J10" s="1" t="s">
         <v>64</v>
@@ -1644,31 +1650,31 @@
         <v>4</v>
       </c>
       <c r="S10" s="1" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="U10" s="1" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="W10" s="1" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="X10" s="1" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="AB10" s="1" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="AC10" s="1" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="AD10" s="1" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="AN10" s="1" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="AR10" s="1" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="AML10" s="1" t="s">
         <v>71</v>
@@ -1676,16 +1682,16 @@
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="C11" s="0" t="s">
         <v>73</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="E11" s="0" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="F11" s="1" t="s">
         <v>76</v>
@@ -1706,19 +1712,16 @@
         <v>4</v>
       </c>
       <c r="S11" s="1" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="U11" s="1" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="W11" s="1" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="X11" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="AB11" s="1" t="s">
-        <v>136</v>
+        <v>80</v>
       </c>
       <c r="AC11" s="1" t="s">
         <v>137</v>
@@ -1727,10 +1730,10 @@
         <v>138</v>
       </c>
       <c r="AN11" s="1" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="AR11" s="1" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="AML11" s="1" t="s">
         <v>71</v>
@@ -1768,16 +1771,16 @@
         <v>5</v>
       </c>
       <c r="S12" s="1" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="U12" s="1" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="W12" s="1" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="X12" s="1" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="AB12" s="1" t="s">
         <v>144</v>
@@ -1830,7 +1833,7 @@
         <v>4</v>
       </c>
       <c r="S13" s="1" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="U13" s="1" t="s">
         <v>152</v>
@@ -1839,7 +1842,7 @@
         <v>153</v>
       </c>
       <c r="X13" s="1" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="AB13" s="1" t="s">
         <v>154</v>
@@ -1865,13 +1868,13 @@
         <v>158</v>
       </c>
       <c r="D14" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="E14" s="0" t="s">
         <v>159</v>
       </c>
-      <c r="E14" s="0" t="s">
+      <c r="F14" s="1" t="s">
         <v>160</v>
-      </c>
-      <c r="F14" s="1" t="s">
-        <v>161</v>
       </c>
       <c r="J14" s="1" t="s">
         <v>64</v>
@@ -1880,7 +1883,7 @@
         <v>536</v>
       </c>
       <c r="P14" s="0" t="n">
-        <v>800</v>
+        <v>2000</v>
       </c>
       <c r="Q14" s="0" t="n">
         <v>0</v>
@@ -1892,25 +1895,28 @@
         <v>65</v>
       </c>
       <c r="U14" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="V14" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="W14" s="1" t="s">
         <v>162</v>
       </c>
-      <c r="W14" s="1" t="s">
+      <c r="X14" s="1" t="s">
         <v>163</v>
       </c>
-      <c r="X14" s="1" t="s">
+      <c r="AB14" s="1" t="s">
         <v>164</v>
       </c>
-      <c r="AB14" s="1" t="s">
+      <c r="AC14" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="AD14" s="1" t="s">
         <v>165</v>
       </c>
-      <c r="AC14" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="AD14" s="1" t="s">
+      <c r="AN14" s="1" t="s">
         <v>166</v>
-      </c>
-      <c r="AN14" s="1" t="s">
-        <v>167</v>
       </c>
       <c r="AR14" s="1" t="s">
         <v>157</v>
@@ -1919,24 +1925,24 @@
         <v>71</v>
       </c>
       <c r="AMM14" s="1" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="C15" s="0" t="s">
         <v>169</v>
       </c>
-      <c r="C15" s="0" t="s">
+      <c r="D15" s="1" t="s">
         <v>170</v>
       </c>
-      <c r="D15" s="1" t="s">
+      <c r="E15" s="0" t="s">
         <v>171</v>
       </c>
-      <c r="E15" s="0" t="s">
+      <c r="F15" s="1" t="s">
         <v>172</v>
-      </c>
-      <c r="F15" s="1" t="s">
-        <v>173</v>
       </c>
       <c r="J15" s="1" t="s">
         <v>64</v>
@@ -1954,22 +1960,28 @@
         <v>4</v>
       </c>
       <c r="S15" s="1" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="U15" s="1" t="s">
         <v>152</v>
       </c>
       <c r="W15" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="X15" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="AB15" s="1" t="s">
         <v>174</v>
       </c>
-      <c r="X15" s="1" t="s">
-        <v>79</v>
+      <c r="AD15" s="1" t="s">
+        <v>175</v>
       </c>
       <c r="AN15" s="1" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="AR15" s="1" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="AML15" s="1" t="s">
         <v>71</v>
@@ -1977,19 +1989,19 @@
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="1" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="C16" s="0" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="E16" s="0" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="J16" s="1" t="s">
         <v>64</v>
@@ -2007,31 +2019,31 @@
         <v>4</v>
       </c>
       <c r="S16" s="1" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="U16" s="1" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="W16" s="1" t="s">
-        <v>78</v>
+        <v>153</v>
       </c>
       <c r="X16" s="1" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="AB16" s="1" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="AC16" s="1" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="AD16" s="1" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="AN16" s="1" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="AR16" s="1" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="AML16" s="1" t="s">
         <v>71</v>
@@ -2039,19 +2051,19 @@
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="1" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="C17" s="0" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="E17" s="0" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="J17" s="1" t="s">
         <v>64</v>
@@ -2069,31 +2081,31 @@
         <v>4</v>
       </c>
       <c r="S17" s="1" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="U17" s="1" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="W17" s="1" t="s">
-        <v>78</v>
+        <v>153</v>
       </c>
       <c r="X17" s="1" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="AB17" s="1" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="AC17" s="1" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="AD17" s="1" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="AN17" s="1" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="AR17" s="1" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="AML17" s="1" t="s">
         <v>71</v>
@@ -2101,19 +2113,19 @@
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="1" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="C18" s="0" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="E18" s="0" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="J18" s="1" t="s">
         <v>64</v>
@@ -2131,31 +2143,31 @@
         <v>4</v>
       </c>
       <c r="S18" s="1" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="U18" s="1" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="W18" s="1" t="s">
-        <v>78</v>
+        <v>153</v>
       </c>
       <c r="X18" s="1" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="AB18" s="1" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="AC18" s="1" t="s">
         <v>137</v>
       </c>
       <c r="AD18" s="1" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="AN18" s="1" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="AR18" s="1" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="AML18" s="1" t="s">
         <v>71</v>
@@ -2163,19 +2175,19 @@
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="1" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="C19" s="0" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="E19" s="0" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="J19" s="1" t="s">
         <v>64</v>
@@ -2193,31 +2205,31 @@
         <v>4</v>
       </c>
       <c r="S19" s="1" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="U19" s="1" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="W19" s="1" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="X19" s="1" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="AB19" s="1" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="AC19" s="1" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="AD19" s="1" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="AN19" s="1" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="AR19" s="1" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="AML19" s="1" t="s">
         <v>71</v>

</xml_diff>